<commit_message>
[Fixed] Subida/Bajada Excel Nóminas
</commit_message>
<xml_diff>
--- a/formatos/formato-nomina.xlsx
+++ b/formatos/formato-nomina.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33256822-270F-49FB-94D6-E6CAE2B92A95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6006073-0283-4E28-B242-9258EBE96B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nominas" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Cargo</t>
-  </si>
-  <si>
     <t>Proceso</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
   </si>
   <si>
     <t>Prestaciones</t>
@@ -53,6 +47,12 @@
   </si>
   <si>
     <t>Tipo de contrato</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Transporte</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1658,37 +1660,37 @@
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="K1" s="9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Fixed] Excel nómina otros ingresos
</commit_message>
<xml_diff>
--- a/formatos/formato-nomina.xlsx
+++ b/formatos/formato-nomina.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6006073-0283-4E28-B242-9258EBE96B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF6C7DC-2A97-4C4A-8741-CE141AA33337}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>Salario</t>
   </si>
   <si>
-    <t>Bonificaciones</t>
-  </si>
-  <si>
     <t>Horas</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>Transporte</t>
+  </si>
+  <si>
+    <t>Otros Ingresos</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1639,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,7 +1660,7 @@
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1669,25 +1669,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>1</v>

</xml_diff>